<commit_message>
Bound some HTML attributes to variables in RSC
</commit_message>
<xml_diff>
--- a/src/assets/files-to-read/example_spreadsheet_large.xlsx
+++ b/src/assets/files-to-read/example_spreadsheet_large.xlsx
@@ -561,7 +561,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -583,6 +583,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -639,7 +645,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -649,6 +655,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,22 +742,40 @@
   <dimension ref="A1:DB15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="AE15" activeCellId="0" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="31.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="1" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="29" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="28.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="26.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="20.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="7.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="31" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="107" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -991,7 +1019,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">

</xml_diff>